<commit_message>
Made it so it adds all the values to the respective classes
</commit_message>
<xml_diff>
--- a/TFTRatios.xlsx
+++ b/TFTRatios.xlsx
@@ -1,17 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\PycharmProjects\TFT\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1960DF-0E2D-4EC6-B2FB-1189BFEE3BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-23235" yWindow="1575" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Position</t>
   </si>
@@ -242,85 +263,123 @@
   </si>
   <si>
     <t>Lock</t>
+  </si>
+  <si>
+    <t>Trove Reroll</t>
+  </si>
+  <si>
+    <t>Trove Pick</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -510,20 +569,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:A48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,1725 +612,1735 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4">
-        <v>560.0</v>
+        <v>560</v>
       </c>
       <c r="C2" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D71" si="1">B2/$G$2</f>
-        <v>0.2916666667</v>
+        <f t="shared" ref="D2:D71" si="0">B2/$G$2</f>
+        <v>0.29166666666666669</v>
       </c>
       <c r="E2" s="4">
-        <f t="shared" ref="E2:E71" si="2">C2/$H$2</f>
-        <v>0.4074074074</v>
+        <f t="shared" ref="E2:E71" si="1">C2/$H$2</f>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="4">
-        <v>1920.0</v>
+        <v>1920</v>
       </c>
       <c r="H2" s="4">
-        <v>1080.0</v>
+        <v>1080</v>
       </c>
       <c r="I2" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4">
-        <v>680.0</v>
+        <v>680</v>
       </c>
       <c r="C3" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3541666667</v>
+        <f t="shared" si="0"/>
+        <v>0.35416666666666669</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="C4" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D4" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4166666667</v>
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="4">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4">
-        <v>920.0</v>
+        <v>920</v>
       </c>
       <c r="C5" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4791666667</v>
+        <f t="shared" si="0"/>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="4">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4">
-        <v>1040.0</v>
+        <v>1040</v>
       </c>
       <c r="C6" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5416666667</v>
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4">
-        <v>1160.0</v>
+        <v>1160</v>
       </c>
       <c r="C7" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6041666667</v>
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4">
-        <v>1280.0</v>
+        <v>1280</v>
       </c>
       <c r="C8" s="4">
-        <v>440.0</v>
+        <v>440</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6666666667</v>
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.40740740740740738</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="4">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4">
-        <v>610.0</v>
+        <v>610</v>
       </c>
       <c r="C9" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3177083333</v>
+        <f t="shared" si="0"/>
+        <v>0.31770833333333331</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="4">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="4">
-        <v>730.0</v>
+        <v>730</v>
       </c>
       <c r="C10" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3802083333</v>
+        <f t="shared" si="0"/>
+        <v>0.38020833333333331</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="4">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="4">
-        <v>850.0</v>
+        <v>850</v>
       </c>
       <c r="C11" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4427083333</v>
+        <f t="shared" si="0"/>
+        <v>0.44270833333333331</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="4">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="4">
-        <v>970.0</v>
+        <v>970</v>
       </c>
       <c r="C12" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5052083333</v>
+        <f t="shared" si="0"/>
+        <v>0.50520833333333337</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="4">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="4">
-        <v>1090.0</v>
+        <v>1090</v>
       </c>
       <c r="C13" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5677083333</v>
+        <f t="shared" si="0"/>
+        <v>0.56770833333333337</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="4">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="4">
-        <v>1210.0</v>
+        <v>1210</v>
       </c>
       <c r="C14" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6302083333</v>
+        <f t="shared" si="0"/>
+        <v>0.63020833333333337</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="4">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="4">
-        <v>1330.0</v>
+        <v>1330</v>
       </c>
       <c r="C15" s="4">
-        <v>515.0</v>
+        <v>515</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6927083333</v>
+        <f t="shared" si="0"/>
+        <v>0.69270833333333337</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="2"/>
-        <v>0.4768518519</v>
+        <f t="shared" si="1"/>
+        <v>0.47685185185185186</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="4">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="4">
-        <v>560.0</v>
+        <v>560</v>
       </c>
       <c r="C16" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2916666667</v>
+        <f t="shared" si="0"/>
+        <v>0.29166666666666669</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="4">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="4">
-        <v>680.0</v>
+        <v>680</v>
       </c>
       <c r="C17" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3541666667</v>
+        <f t="shared" si="0"/>
+        <v>0.35416666666666669</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="4">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="4">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="C18" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4166666667</v>
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="4">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="4">
-        <v>920.0</v>
+        <v>920</v>
       </c>
       <c r="C19" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4791666667</v>
+        <f t="shared" si="0"/>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="4">
-        <v>17.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="4">
-        <v>1040.0</v>
+        <v>1040</v>
       </c>
       <c r="C20" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5416666667</v>
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="4">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="4">
-        <v>1160.0</v>
+        <v>1160</v>
       </c>
       <c r="C21" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6041666667</v>
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="4">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="4">
-        <v>1280.0</v>
+        <v>1280</v>
       </c>
       <c r="C22" s="4">
-        <v>590.0</v>
+        <v>590</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6666666667</v>
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5462962963</v>
+        <f t="shared" si="1"/>
+        <v>0.54629629629629628</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="4">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="4">
-        <v>610.0</v>
+        <v>610</v>
       </c>
       <c r="C23" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3177083333</v>
+        <f t="shared" si="0"/>
+        <v>0.31770833333333331</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="4">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="4">
-        <v>730.0</v>
+        <v>730</v>
       </c>
       <c r="C24" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3802083333</v>
+        <f t="shared" si="0"/>
+        <v>0.38020833333333331</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="4">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="4">
-        <v>850.0</v>
+        <v>850</v>
       </c>
       <c r="C25" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4427083333</v>
+        <f t="shared" si="0"/>
+        <v>0.44270833333333331</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="4">
-        <v>23.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="4">
-        <v>970.0</v>
+        <v>970</v>
       </c>
       <c r="C26" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5052083333</v>
+        <f t="shared" si="0"/>
+        <v>0.50520833333333337</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="4">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="4">
-        <v>1090.0</v>
+        <v>1090</v>
       </c>
       <c r="C27" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5677083333</v>
+        <f t="shared" si="0"/>
+        <v>0.56770833333333337</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="4">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="4">
-        <v>1210.0</v>
+        <v>1210</v>
       </c>
       <c r="C28" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6302083333</v>
+        <f t="shared" si="0"/>
+        <v>0.63020833333333337</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="4">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="4">
-        <v>1330.0</v>
+        <v>1330</v>
       </c>
       <c r="C29" s="4">
-        <v>665.0</v>
+        <v>665</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6927083333</v>
+        <f t="shared" si="0"/>
+        <v>0.69270833333333337</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6157407407</v>
+        <f t="shared" si="1"/>
+        <v>0.6157407407407407</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="4">
-        <v>27.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="4">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="C30" s="4">
-        <v>645.0</v>
+        <v>645</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1666666667</v>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5972222222</v>
+        <f t="shared" si="1"/>
+        <v>0.59722222222222221</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="4">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B31" s="4">
-        <v>370.0</v>
+        <v>370</v>
       </c>
       <c r="C31" s="4">
-        <v>645.0</v>
+        <v>645</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1927083333</v>
+        <f t="shared" si="0"/>
+        <v>0.19270833333333334</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5972222222</v>
+        <f t="shared" si="1"/>
+        <v>0.59722222222222221</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="4">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B32" s="4">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="C32" s="4">
-        <v>685.0</v>
+        <v>685</v>
       </c>
       <c r="D32" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1588541667</v>
+        <f t="shared" si="0"/>
+        <v>0.15885416666666666</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6342592593</v>
+        <f t="shared" si="1"/>
+        <v>0.6342592592592593</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="4">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B33" s="4">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="C33" s="4">
-        <v>685.0</v>
+        <v>685</v>
       </c>
       <c r="D33" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6342592593</v>
+        <f t="shared" si="1"/>
+        <v>0.6342592592592593</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="4">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B34" s="4">
-        <v>415.0</v>
+        <v>415</v>
       </c>
       <c r="C34" s="4">
-        <v>685.0</v>
+        <v>685</v>
       </c>
       <c r="D34" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2161458333</v>
+        <f t="shared" si="0"/>
+        <v>0.21614583333333334</v>
       </c>
       <c r="E34" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6342592593</v>
+        <f t="shared" si="1"/>
+        <v>0.6342592592592593</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="4">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="4">
-        <v>325.0</v>
+        <v>325</v>
       </c>
       <c r="C35" s="4">
-        <v>715.0</v>
+        <v>715</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1692708333</v>
+        <f t="shared" si="0"/>
+        <v>0.16927083333333334</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="2"/>
-        <v>0.662037037</v>
+        <f t="shared" si="1"/>
+        <v>0.66203703703703709</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="4">
-        <v>33.0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="4">
-        <v>380.0</v>
+        <v>380</v>
       </c>
       <c r="C36" s="4">
-        <v>715.0</v>
+        <v>715</v>
       </c>
       <c r="D36" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1979166667</v>
+        <f t="shared" si="0"/>
+        <v>0.19791666666666666</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="2"/>
-        <v>0.662037037</v>
+        <f t="shared" si="1"/>
+        <v>0.66203703703703709</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="4">
-        <v>34.0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="4">
-        <v>280.0</v>
+        <v>280</v>
       </c>
       <c r="C37" s="4">
-        <v>745.0</v>
+        <v>745</v>
       </c>
       <c r="D37" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1458333333</v>
+        <f t="shared" si="0"/>
+        <v>0.14583333333333334</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="2"/>
-        <v>0.6898148148</v>
+        <f t="shared" si="1"/>
+        <v>0.68981481481481477</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="4">
-        <v>35.0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B38" s="4">
-        <v>310.0</v>
+        <v>310</v>
       </c>
       <c r="C38" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D38" s="4">
-        <f t="shared" si="1"/>
-        <v>0.1614583333</v>
+        <f t="shared" si="0"/>
+        <v>0.16145833333333334</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="4">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B39" s="4">
-        <v>270.0</v>
+        <v>270</v>
       </c>
       <c r="C39" s="4">
-        <v>810.0</v>
+        <v>810</v>
       </c>
       <c r="D39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.140625</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="I39" s="4">
-        <v>37.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B40" s="4">
-        <v>420.0</v>
+        <v>420</v>
       </c>
       <c r="C40" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.21875</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G40" s="2"/>
       <c r="I40" s="4">
-        <v>38.0</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="4">
-        <v>540.0</v>
+        <v>540</v>
       </c>
       <c r="C41" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D41" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.28125</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G41" s="2"/>
       <c r="I41" s="4">
-        <v>39.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="4">
-        <v>660.0</v>
+        <v>660</v>
       </c>
       <c r="C42" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D42" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.34375</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G42" s="2"/>
       <c r="I42" s="4">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="C43" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.40625</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G43" s="2"/>
       <c r="I43" s="4">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="4">
-        <v>900.0</v>
+        <v>900</v>
       </c>
       <c r="C44" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.46875</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G44" s="2"/>
       <c r="I44" s="4">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="4">
-        <v>1020.0</v>
+        <v>1020</v>
       </c>
       <c r="C45" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D45" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.53125</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G45" s="2"/>
       <c r="I45" s="4">
-        <v>43.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="4">
-        <v>1140.0</v>
+        <v>1140</v>
       </c>
       <c r="C46" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D46" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.59375</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G46" s="2"/>
       <c r="I46" s="4">
-        <v>44.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B47" s="4">
-        <v>1260.0</v>
+        <v>1260</v>
       </c>
       <c r="C47" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="D47" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.65625</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G47" s="2"/>
       <c r="I47" s="4">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="6">
-        <v>1380.0</v>
-      </c>
-      <c r="C48" s="6">
-        <v>780.0</v>
+      <c r="B48" s="5">
+        <v>1380</v>
+      </c>
+      <c r="C48" s="5">
+        <v>780</v>
       </c>
       <c r="D48" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.71875</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="2"/>
-        <v>0.7222222222</v>
+        <f t="shared" si="1"/>
+        <v>0.72222222222222221</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="4">
-        <v>46.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B49" s="4">
-        <v>580.0</v>
+        <v>580</v>
       </c>
       <c r="C49" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D49" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3020833333</v>
+        <f t="shared" si="0"/>
+        <v>0.30208333333333331</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="4">
-        <v>47.0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="4">
-        <v>780.0</v>
+        <v>780</v>
       </c>
       <c r="C50" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D50" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.40625</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="4">
-        <v>48.0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B51" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="C51" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D51" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5104166667</v>
+        <f t="shared" si="0"/>
+        <v>0.51041666666666663</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="4">
-        <v>49.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="4">
-        <v>1180.0</v>
+        <v>1180</v>
       </c>
       <c r="C52" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6145833333</v>
+        <f t="shared" si="0"/>
+        <v>0.61458333333333337</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="4">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
         <v>58</v>
       </c>
       <c r="B53" s="4">
-        <v>1380.0</v>
+        <v>1380</v>
       </c>
       <c r="C53" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.71875</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="4">
-        <v>51.0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B54" s="4">
-        <v>520.0</v>
+        <v>520</v>
       </c>
       <c r="C54" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D54" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2708333333</v>
+        <f t="shared" si="0"/>
+        <v>0.27083333333333331</v>
       </c>
       <c r="E54" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="4">
-        <v>52.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B55" s="4">
-        <v>760.0</v>
+        <v>760</v>
       </c>
       <c r="C55" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D55" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3958333333</v>
+        <f t="shared" si="0"/>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E55" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="4">
-        <v>53.0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B56" s="4">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="C56" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D56" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5208333333</v>
+        <f t="shared" si="0"/>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="4">
-        <v>54.0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B57" s="4">
-        <v>1240.0</v>
+        <v>1240</v>
       </c>
       <c r="C57" s="4">
-        <v>980.0</v>
+        <v>980</v>
       </c>
       <c r="D57" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6458333333</v>
+        <f t="shared" si="0"/>
+        <v>0.64583333333333337</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="4">
-        <v>55.0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="4">
-        <v>580.0</v>
+        <v>580</v>
       </c>
       <c r="C58" s="4">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="D58" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3020833333</v>
+        <f t="shared" si="0"/>
+        <v>0.30208333333333331</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5555555556</v>
+        <f t="shared" si="1"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="4">
-        <v>56.0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B59" s="4">
-        <v>950.0</v>
+        <v>950</v>
       </c>
       <c r="C59" s="4">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="D59" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4947916667</v>
+        <f t="shared" si="0"/>
+        <v>0.49479166666666669</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5555555556</v>
+        <f t="shared" si="1"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="4">
-        <v>57.0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B60" s="4">
-        <v>1300.0</v>
+        <v>1300</v>
       </c>
       <c r="C60" s="4">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="D60" s="4">
-        <f t="shared" si="1"/>
-        <v>0.6770833333</v>
+        <f t="shared" si="0"/>
+        <v>0.67708333333333337</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="2"/>
-        <v>0.5555555556</v>
+        <f t="shared" si="1"/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="4">
-        <v>58.0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="4">
-        <v>560.0</v>
+        <v>560</v>
       </c>
       <c r="C61" s="4">
-        <v>930.0</v>
+        <v>930</v>
       </c>
       <c r="D61" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2916666667</v>
+        <f t="shared" si="0"/>
+        <v>0.29166666666666669</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" si="2"/>
-        <v>0.8611111111</v>
+        <f t="shared" si="1"/>
+        <v>0.86111111111111116</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="4">
-        <v>59.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="4">
-        <v>760.0</v>
+        <v>760</v>
       </c>
       <c r="C62" s="4">
-        <v>930.0</v>
+        <v>930</v>
       </c>
       <c r="D62" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3958333333</v>
+        <f t="shared" si="0"/>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="2"/>
-        <v>0.8611111111</v>
+        <f t="shared" si="1"/>
+        <v>0.86111111111111116</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="4">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="4">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="C63" s="4">
-        <v>930.0</v>
+        <v>930</v>
       </c>
       <c r="D63" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" si="2"/>
-        <v>0.8611111111</v>
+        <f t="shared" si="1"/>
+        <v>0.86111111111111116</v>
       </c>
       <c r="I63" s="4">
-        <v>61.0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B64" s="6">
-        <v>400.0</v>
-      </c>
-      <c r="C64" s="6">
-        <v>980.0</v>
+      <c r="B64" s="5">
+        <v>400</v>
+      </c>
+      <c r="C64" s="5">
+        <v>980</v>
       </c>
       <c r="D64" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2083333333</v>
+        <f t="shared" si="0"/>
+        <v>0.20833333333333334</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="I64" s="4">
-        <v>62.0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B65" s="6">
-        <v>640.0</v>
-      </c>
-      <c r="C65" s="6">
-        <v>980.0</v>
+      <c r="B65" s="5">
+        <v>640</v>
+      </c>
+      <c r="C65" s="5">
+        <v>980</v>
       </c>
       <c r="D65" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3333333333</v>
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E65" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="I65" s="4">
-        <v>63.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B66" s="6">
-        <v>880.0</v>
-      </c>
-      <c r="C66" s="6">
-        <v>980.0</v>
+      <c r="B66" s="5">
+        <v>880</v>
+      </c>
+      <c r="C66" s="5">
+        <v>980</v>
       </c>
       <c r="D66" s="4">
-        <f t="shared" si="1"/>
-        <v>0.4583333333</v>
+        <f t="shared" si="0"/>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E66" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
-      <c r="I66" s="6">
-        <v>64.0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="6" t="s">
+      <c r="I66" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B67" s="6">
-        <v>1120.0</v>
-      </c>
-      <c r="C67" s="6">
-        <v>980.0</v>
+      <c r="B67" s="5">
+        <v>1120</v>
+      </c>
+      <c r="C67" s="5">
+        <v>980</v>
       </c>
       <c r="D67" s="4">
-        <f t="shared" si="1"/>
-        <v>0.5833333333</v>
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
-      <c r="I67" s="6">
-        <v>65.0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="6" t="s">
+      <c r="I67" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="6">
-        <v>1480.0</v>
-      </c>
-      <c r="C68" s="6">
-        <v>980.0</v>
+      <c r="B68" s="5">
+        <v>1480</v>
+      </c>
+      <c r="C68" s="5">
+        <v>980</v>
       </c>
       <c r="D68" s="4">
-        <f t="shared" si="1"/>
-        <v>0.7708333333</v>
+        <f t="shared" si="0"/>
+        <v>0.77083333333333337</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" si="2"/>
-        <v>0.9074074074</v>
+        <f t="shared" si="1"/>
+        <v>0.90740740740740744</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
-      <c r="I68" s="6">
-        <v>66.0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="s">
+      <c r="I68" s="5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="4">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="C69" s="4">
-        <v>960.0</v>
+        <v>960</v>
       </c>
       <c r="D69" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="2"/>
-        <v>0.8888888889</v>
-      </c>
-      <c r="I69" s="6">
-        <v>67.0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="I69" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" s="9" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="4">
-        <v>360.0</v>
+        <v>360</v>
       </c>
       <c r="C70" s="4">
-        <v>1040.0</v>
+        <v>1040</v>
       </c>
       <c r="D70" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.1875</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="2"/>
-        <v>0.962962963</v>
-      </c>
-      <c r="I70" s="6">
-        <v>68.0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="s">
+        <f t="shared" si="1"/>
+        <v>0.96296296296296291</v>
+      </c>
+      <c r="I70" s="5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="4">
-        <v>1450.0</v>
+        <v>1450</v>
       </c>
       <c r="C71" s="4">
-        <v>905.0</v>
+        <v>905</v>
       </c>
       <c r="D71" s="4">
-        <f t="shared" si="1"/>
-        <v>0.7552083333</v>
+        <f t="shared" si="0"/>
+        <v>0.75520833333333337</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="2"/>
-        <v>0.837962963</v>
-      </c>
-      <c r="I71" s="6">
-        <v>69.0</v>
+        <f t="shared" si="1"/>
+        <v>0.83796296296296291</v>
+      </c>
+      <c r="I71" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up some of the code
</commit_message>
<xml_diff>
--- a/TFTRatios.xlsx
+++ b/TFTRatios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\PycharmProjects\TFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1960DF-0E2D-4EC6-B2FB-1189BFEE3BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4FFB6D-D1CF-496B-8B60-FF0AE54F48AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23235" yWindow="1575" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -211,51 +211,6 @@
     <t>Buy5</t>
   </si>
   <si>
-    <t>Tome 1</t>
-  </si>
-  <si>
-    <t>Tome 2</t>
-  </si>
-  <si>
-    <t>Tome 3</t>
-  </si>
-  <si>
-    <t>Tome 4</t>
-  </si>
-  <si>
-    <t>Augment 1</t>
-  </si>
-  <si>
-    <t>Augment 2</t>
-  </si>
-  <si>
-    <t>Augment 3</t>
-  </si>
-  <si>
-    <t>Armory 1</t>
-  </si>
-  <si>
-    <t>Armory 2</t>
-  </si>
-  <si>
-    <t>Armory 3</t>
-  </si>
-  <si>
-    <t>Radiant 1</t>
-  </si>
-  <si>
-    <t>Radiant 2</t>
-  </si>
-  <si>
-    <t>Radiant 3</t>
-  </si>
-  <si>
-    <t>Radiant 4</t>
-  </si>
-  <si>
-    <t>Radiant 5</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -269,6 +224,51 @@
   </si>
   <si>
     <t>Trove Pick</t>
+  </si>
+  <si>
+    <t>Tome1</t>
+  </si>
+  <si>
+    <t>Tome2</t>
+  </si>
+  <si>
+    <t>Tome3</t>
+  </si>
+  <si>
+    <t>Tome4</t>
+  </si>
+  <si>
+    <t>Augment1</t>
+  </si>
+  <si>
+    <t>Augment2</t>
+  </si>
+  <si>
+    <t>Augment3</t>
+  </si>
+  <si>
+    <t>Armory1</t>
+  </si>
+  <si>
+    <t>Armory2</t>
+  </si>
+  <si>
+    <t>Armory3</t>
+  </si>
+  <si>
+    <t>Radiant1</t>
+  </si>
+  <si>
+    <t>Radiant2</t>
+  </si>
+  <si>
+    <t>Radiant3</t>
+  </si>
+  <si>
+    <t>Radiant4</t>
+  </si>
+  <si>
+    <t>Radiant5</t>
   </si>
 </sst>
 </file>
@@ -579,15 +579,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:A48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +612,7 @@
       </c>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
@@ -716,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -766,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -791,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -816,7 +816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -841,7 +841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -866,7 +866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -891,7 +891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -916,7 +916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
@@ -941,7 +941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
@@ -966,7 +966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -991,7 +991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>33</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>34</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>36</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>37</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>40</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>41</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>42</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>43</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>44</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>51</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>52</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>53</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>54</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
         <v>55</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>56</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
         <v>57</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>58</v>
       </c>
@@ -1898,9 +1898,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B54" s="4">
         <v>520</v>
@@ -1923,9 +1923,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B55" s="4">
         <v>760</v>
@@ -1948,9 +1948,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B56" s="4">
         <v>1000</v>
@@ -1973,9 +1973,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B57" s="4">
         <v>1240</v>
@@ -1998,9 +1998,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B58" s="4">
         <v>580</v>
@@ -2023,9 +2023,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B59" s="4">
         <v>950</v>
@@ -2048,9 +2048,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B60" s="4">
         <v>1300</v>
@@ -2073,9 +2073,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B61" s="4">
         <v>560</v>
@@ -2098,9 +2098,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B62" s="4">
         <v>760</v>
@@ -2123,9 +2123,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B63" s="4">
         <v>960</v>
@@ -2145,9 +2145,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B64" s="5">
         <v>400</v>
@@ -2167,9 +2167,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B65" s="5">
         <v>640</v>
@@ -2189,9 +2189,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B66" s="5">
         <v>880</v>
@@ -2214,9 +2214,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B67" s="5">
         <v>1120</v>
@@ -2239,9 +2239,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B68" s="5">
         <v>1480</v>
@@ -2263,10 +2263,13 @@
       <c r="I68" s="5">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N68" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B69" s="4">
         <v>360</v>
@@ -2285,10 +2288,13 @@
       <c r="I69" s="5">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N69" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B70" s="4">
         <v>360</v>
@@ -2308,9 +2314,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B71" s="4">
         <v>1450</v>
@@ -2328,16 +2334,6 @@
       </c>
       <c r="I71" s="5">
         <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>